<commit_message>
Added LCSC BOM for PCBWay
</commit_message>
<xml_diff>
--- a/Production/BOMs/PCBWay/3DProUsb-PCBWay-BOM-LCSC.xlsx
+++ b/Production/BOMs/PCBWay/3DProUsb-PCBWay-BOM-LCSC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kreeblah/SidewinderToUSBV2/Production/BOMs/PCBWay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92F20AD-4341-CA4D-9BFC-37901A2D37DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5893890E-E513-7845-8B16-E282411D5DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,9 +174,6 @@
     <t>Microchip Technology</t>
   </si>
   <si>
-    <t>ATMEGA32U4-MU</t>
-  </si>
-  <si>
     <t>IC MCU 8BIT 32KB FLASH 44VQFN</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>LCSC Part: C231481</t>
   </si>
   <si>
-    <t>LCSC Part: C112161</t>
-  </si>
-  <si>
     <t>Suzhou Liming Elec</t>
   </si>
   <si>
@@ -364,6 +358,12 @@
   </si>
   <si>
     <t>LCSC Part: C479112</t>
+  </si>
+  <si>
+    <t>ATMEGA32U4-MUR</t>
+  </si>
+  <si>
+    <t>LCSC Part: C45874</t>
   </si>
 </sst>
 </file>
@@ -950,7 +950,7 @@
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="D2" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
@@ -1019,10 +1019,10 @@
         <v>10</v>
       </c>
       <c r="H7" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1">
@@ -1030,28 +1030,28 @@
         <v>2</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
       </c>
       <c r="D8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="F8" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="G8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>32</v>
-      </c>
       <c r="H8" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1059,28 +1059,28 @@
         <v>3</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
       </c>
       <c r="D9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="F9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1097,11 +1097,11 @@
         <v>25</v>
       </c>
       <c r="E10" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>27</v>
-      </c>
       <c r="G10" s="8" t="s">
         <v>10</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>10</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1117,28 +1117,28 @@
         <v>5</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="22">
         <v>1</v>
       </c>
       <c r="D11" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1146,20 +1146,20 @@
         <v>6</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="22">
         <v>1</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>40</v>
-      </c>
       <c r="G12" s="23" t="s">
         <v>10</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>10</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1175,28 +1175,28 @@
         <v>7</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="22">
         <v>1</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="21" t="s">
         <v>64</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1210,10 +1210,10 @@
         <v>2</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>17</v>
@@ -1225,7 +1225,7 @@
         <v>10</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1239,10 +1239,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>20</v>
@@ -1254,7 +1254,7 @@
         <v>10</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1">
@@ -1268,10 +1268,10 @@
         <v>2</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>22</v>
@@ -1283,7 +1283,7 @@
         <v>10</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1297,10 +1297,10 @@
         <v>2</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>24</v>
@@ -1312,7 +1312,7 @@
         <v>10</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1320,19 +1320,19 @@
         <v>12</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="13">
         <v>2</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>18</v>
@@ -1341,7 +1341,7 @@
         <v>10</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1349,19 +1349,19 @@
         <v>13</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>18</v>
@@ -1370,7 +1370,7 @@
         <v>10</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1378,19 +1378,19 @@
         <v>14</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="13">
         <v>2</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>18</v>
@@ -1399,7 +1399,7 @@
         <v>10</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1407,28 +1407,28 @@
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="13">
         <v>1</v>
       </c>
       <c r="D21" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:9">

</xml_diff>

<commit_message>
Updated BOMs and README for tested board.
</commit_message>
<xml_diff>
--- a/Production/BOMs/PCBWay/3DProUsb-PCBWay-BOM-LCSC.xlsx
+++ b/Production/BOMs/PCBWay/3DProUsb-PCBWay-BOM-LCSC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kreeblah/SidewinderToUSBV2/Production/BOMs/PCBWay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EF504B-DD75-4049-A3B8-325365857BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1906A2E4-4777-2141-BF37-479E9D3FEA40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
   <si>
     <t>Item #</t>
   </si>
@@ -255,12 +255,6 @@
     <t>Omron Electronics</t>
   </si>
   <si>
-    <t>XM3B-1522-502</t>
-  </si>
-  <si>
-    <t>LCSC Part: C231481</t>
-  </si>
-  <si>
     <t>Suzhou Liming Elec</t>
   </si>
   <si>
@@ -367,6 +361,15 @@
   </si>
   <si>
     <t>LCSC Part: C132562</t>
+  </si>
+  <si>
+    <t>CONNFLY Elec</t>
+  </si>
+  <si>
+    <t>DS1037-15FNAKT74-0CC</t>
+  </si>
+  <si>
+    <t>LCSC Part: C77835</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1013,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>14</v>
@@ -1025,7 +1028,7 @@
         <v>51</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1">
@@ -1068,10 +1071,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>31</v>
@@ -1083,7 +1086,7 @@
         <v>50</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1100,7 +1103,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>24</v>
@@ -1112,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1126,10 +1129,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" s="21" t="s">
         <v>34</v>
@@ -1141,7 +1144,7 @@
         <v>10</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1170,7 +1173,7 @@
         <v>10</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1184,10 +1187,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>39</v>
@@ -1199,7 +1202,7 @@
         <v>10</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1207,16 +1210,16 @@
         <v>8</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C14" s="15">
         <v>3</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>15</v>
@@ -1228,7 +1231,7 @@
         <v>10</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1242,10 +1245,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>18</v>
@@ -1257,7 +1260,7 @@
         <v>10</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1">
@@ -1271,10 +1274,10 @@
         <v>2</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>20</v>
@@ -1286,7 +1289,7 @@
         <v>10</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1300,10 +1303,10 @@
         <v>2</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>22</v>
@@ -1315,7 +1318,7 @@
         <v>10</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1329,10 +1332,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>42</v>
@@ -1344,7 +1347,7 @@
         <v>10</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1358,10 +1361,10 @@
         <v>2</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>43</v>
@@ -1373,7 +1376,7 @@
         <v>10</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1387,10 +1390,10 @@
         <v>2</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>46</v>
@@ -1402,7 +1405,7 @@
         <v>10</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1416,13 +1419,13 @@
         <v>1</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>48</v>
@@ -1431,7 +1434,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:9">

</xml_diff>